<commit_message>
Changes to SoBCalCbIC, ElaE, WMITR, based on India data updates from Deepthi and new US EPS additions - ICpUEfEBE and Cross-Sec-Tot
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
+++ b/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\SoBCaICbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\SoBCaICbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A568A-4A9A-4A92-8DE0-40083EE19C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1290" windowWidth="24765" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1290" windowWidth="24765" windowHeight="16080" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -34,7 +33,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="14">TableB42!$2:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="12">TableB44!$2:$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2193,12 +2192,6 @@
     <t>Other equipment includes primarily additional plug load equipment including computers and televisions</t>
   </si>
   <si>
-    <t>We assume all other equipment are direct purchase without install</t>
-  </si>
-  <si>
-    <t>Mostly likely to be TVs, computers, and monitors</t>
-  </si>
-  <si>
     <t>Note from "Updated Building Sector Appliance and Equipment Costs and Efficiencies."</t>
   </si>
   <si>
@@ -2212,12 +2205,18 @@
   </si>
   <si>
     <t>Unit: dimensionless (%)</t>
+  </si>
+  <si>
+    <t>We use the same breakdown as for appliances for</t>
+  </si>
+  <si>
+    <t>the other equipment category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -3019,15 +3018,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Body: normal cell" xfId="6"/>
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="8"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Parent row" xfId="7"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Table title" xfId="4"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -3325,10 +3324,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3341,7 +3340,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,17 +3455,17 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="114" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="113" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="113" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -3503,10 +3502,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1" location="/?id=30-AEO2020&amp;cases=ref2020&amp;sourcekey=0" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B14" r:id="rId3" location="b38-b46" display="https://www.eia.gov/consumption/commercial/data/2012/ - b38-b46" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B21" r:id="rId1" location="/?id=30-AEO2020&amp;cases=ref2020&amp;sourcekey=0"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B14" r:id="rId3" location="b38-b46" display="https://www.eia.gov/consumption/commercial/data/2012/ - b38-b46"/>
+    <hyperlink ref="B28" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -3514,7 +3513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -3529,7 +3528,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -4451,7 +4450,7 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
@@ -4475,7 +4474,7 @@
       </c>
       <c r="W7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
@@ -4540,7 +4539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -4555,7 +4554,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -5477,7 +5476,7 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
@@ -5501,7 +5500,7 @@
       </c>
       <c r="W7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
@@ -5566,7 +5565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N202"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11903,7 +11902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K190"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17331,7 +17330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25220,14 +25219,14 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="/?id=30-AEO2020&amp;cases=ref2020&amp;sourcekey=0" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" location="/?id=30-AEO2020&amp;cases=ref2020&amp;sourcekey=0"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -30938,7 +30937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -31261,7 +31260,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31357,7 +31356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -33280,101 +33279,101 @@
     <mergeCell ref="A43:H43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="H8" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="H13" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="H14" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="H15" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="H16" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="H17" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="H18" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="H19" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="H20" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="H21" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="H22" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
-    <hyperlink ref="H23" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
-    <hyperlink ref="H24" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
-    <hyperlink ref="H25" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
-    <hyperlink ref="H26" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
-    <hyperlink ref="H27" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
-    <hyperlink ref="H28" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
-    <hyperlink ref="H29" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
-    <hyperlink ref="H30" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
-    <hyperlink ref="H31" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
-    <hyperlink ref="H32" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
-    <hyperlink ref="H33" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
-    <hyperlink ref="H35" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
-    <hyperlink ref="H36" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
-    <hyperlink ref="H37" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
-    <hyperlink ref="H38" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
-    <hyperlink ref="H39" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
-    <hyperlink ref="H45" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
-    <hyperlink ref="H46" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
-    <hyperlink ref="H47" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
-    <hyperlink ref="H48" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
-    <hyperlink ref="H49" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
-    <hyperlink ref="H50" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
-    <hyperlink ref="H51" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
-    <hyperlink ref="H52" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
-    <hyperlink ref="H53" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
-    <hyperlink ref="H54" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
-    <hyperlink ref="H55" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
-    <hyperlink ref="H56" r:id="rId47" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
-    <hyperlink ref="H57" r:id="rId48" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
-    <hyperlink ref="H58" r:id="rId49" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
-    <hyperlink ref="H59" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
-    <hyperlink ref="H60" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
-    <hyperlink ref="H61" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
-    <hyperlink ref="H62" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
-    <hyperlink ref="H63" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
-    <hyperlink ref="H64" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
-    <hyperlink ref="H65" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
-    <hyperlink ref="H66" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
-    <hyperlink ref="H67" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
-    <hyperlink ref="H68" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
-    <hyperlink ref="H69" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
-    <hyperlink ref="H70" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
-    <hyperlink ref="H71" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003D000000}"/>
-    <hyperlink ref="H72" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
-    <hyperlink ref="H73" r:id="rId64" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
-    <hyperlink ref="H74" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
-    <hyperlink ref="H75" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
-    <hyperlink ref="H76" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
-    <hyperlink ref="H77" r:id="rId68" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
-    <hyperlink ref="H78" r:id="rId69" xr:uid="{00000000-0004-0000-0300-000044000000}"/>
-    <hyperlink ref="H79" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
-    <hyperlink ref="H80" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
-    <hyperlink ref="H81" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
-    <hyperlink ref="H82" r:id="rId73" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
-    <hyperlink ref="H83" r:id="rId74" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
-    <hyperlink ref="H84" r:id="rId75" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
-    <hyperlink ref="H85" r:id="rId76" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
-    <hyperlink ref="H86" r:id="rId77" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
-    <hyperlink ref="H87" r:id="rId78" xr:uid="{00000000-0004-0000-0300-00004D000000}"/>
-    <hyperlink ref="H88" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00004E000000}"/>
-    <hyperlink ref="H89" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00004F000000}"/>
-    <hyperlink ref="H90" r:id="rId81" xr:uid="{00000000-0004-0000-0300-000050000000}"/>
-    <hyperlink ref="H91" r:id="rId82" xr:uid="{00000000-0004-0000-0300-000051000000}"/>
-    <hyperlink ref="H92" r:id="rId83" xr:uid="{00000000-0004-0000-0300-000052000000}"/>
-    <hyperlink ref="H93" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000053000000}"/>
-    <hyperlink ref="H94" r:id="rId85" xr:uid="{00000000-0004-0000-0300-000054000000}"/>
-    <hyperlink ref="H95" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
-    <hyperlink ref="H96" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
-    <hyperlink ref="H97" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000057000000}"/>
-    <hyperlink ref="H98" r:id="rId89" xr:uid="{00000000-0004-0000-0300-000058000000}"/>
-    <hyperlink ref="H99" r:id="rId90" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
-    <hyperlink ref="H100" r:id="rId91" xr:uid="{00000000-0004-0000-0300-00005A000000}"/>
-    <hyperlink ref="H101" r:id="rId92" xr:uid="{00000000-0004-0000-0300-00005B000000}"/>
-    <hyperlink ref="H102" r:id="rId93" xr:uid="{00000000-0004-0000-0300-00005C000000}"/>
-    <hyperlink ref="H103" r:id="rId94" xr:uid="{00000000-0004-0000-0300-00005D000000}"/>
-    <hyperlink ref="H104" r:id="rId95" xr:uid="{00000000-0004-0000-0300-00005E000000}"/>
+    <hyperlink ref="H4" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
+    <hyperlink ref="H9" r:id="rId6"/>
+    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="H11" r:id="rId8"/>
+    <hyperlink ref="H12" r:id="rId9"/>
+    <hyperlink ref="H13" r:id="rId10"/>
+    <hyperlink ref="H14" r:id="rId11"/>
+    <hyperlink ref="H15" r:id="rId12"/>
+    <hyperlink ref="H16" r:id="rId13"/>
+    <hyperlink ref="H17" r:id="rId14"/>
+    <hyperlink ref="H18" r:id="rId15"/>
+    <hyperlink ref="H19" r:id="rId16"/>
+    <hyperlink ref="H20" r:id="rId17"/>
+    <hyperlink ref="H21" r:id="rId18"/>
+    <hyperlink ref="H22" r:id="rId19"/>
+    <hyperlink ref="H23" r:id="rId20"/>
+    <hyperlink ref="H24" r:id="rId21"/>
+    <hyperlink ref="H25" r:id="rId22"/>
+    <hyperlink ref="H26" r:id="rId23"/>
+    <hyperlink ref="H27" r:id="rId24"/>
+    <hyperlink ref="H28" r:id="rId25"/>
+    <hyperlink ref="H29" r:id="rId26"/>
+    <hyperlink ref="H30" r:id="rId27"/>
+    <hyperlink ref="H31" r:id="rId28"/>
+    <hyperlink ref="H32" r:id="rId29"/>
+    <hyperlink ref="H33" r:id="rId30"/>
+    <hyperlink ref="H35" r:id="rId31"/>
+    <hyperlink ref="H36" r:id="rId32"/>
+    <hyperlink ref="H37" r:id="rId33"/>
+    <hyperlink ref="H38" r:id="rId34"/>
+    <hyperlink ref="H39" r:id="rId35"/>
+    <hyperlink ref="H45" r:id="rId36"/>
+    <hyperlink ref="H46" r:id="rId37"/>
+    <hyperlink ref="H47" r:id="rId38"/>
+    <hyperlink ref="H48" r:id="rId39"/>
+    <hyperlink ref="H49" r:id="rId40"/>
+    <hyperlink ref="H50" r:id="rId41"/>
+    <hyperlink ref="H51" r:id="rId42"/>
+    <hyperlink ref="H52" r:id="rId43"/>
+    <hyperlink ref="H53" r:id="rId44"/>
+    <hyperlink ref="H54" r:id="rId45"/>
+    <hyperlink ref="H55" r:id="rId46"/>
+    <hyperlink ref="H56" r:id="rId47"/>
+    <hyperlink ref="H57" r:id="rId48"/>
+    <hyperlink ref="H58" r:id="rId49"/>
+    <hyperlink ref="H59" r:id="rId50"/>
+    <hyperlink ref="H60" r:id="rId51"/>
+    <hyperlink ref="H61" r:id="rId52"/>
+    <hyperlink ref="H62" r:id="rId53"/>
+    <hyperlink ref="H63" r:id="rId54"/>
+    <hyperlink ref="H64" r:id="rId55"/>
+    <hyperlink ref="H65" r:id="rId56"/>
+    <hyperlink ref="H66" r:id="rId57"/>
+    <hyperlink ref="H67" r:id="rId58"/>
+    <hyperlink ref="H68" r:id="rId59"/>
+    <hyperlink ref="H69" r:id="rId60"/>
+    <hyperlink ref="H70" r:id="rId61"/>
+    <hyperlink ref="H71" r:id="rId62"/>
+    <hyperlink ref="H72" r:id="rId63"/>
+    <hyperlink ref="H73" r:id="rId64"/>
+    <hyperlink ref="H74" r:id="rId65"/>
+    <hyperlink ref="H75" r:id="rId66"/>
+    <hyperlink ref="H76" r:id="rId67"/>
+    <hyperlink ref="H77" r:id="rId68"/>
+    <hyperlink ref="H78" r:id="rId69"/>
+    <hyperlink ref="H79" r:id="rId70"/>
+    <hyperlink ref="H80" r:id="rId71"/>
+    <hyperlink ref="H81" r:id="rId72"/>
+    <hyperlink ref="H82" r:id="rId73"/>
+    <hyperlink ref="H83" r:id="rId74"/>
+    <hyperlink ref="H84" r:id="rId75"/>
+    <hyperlink ref="H85" r:id="rId76"/>
+    <hyperlink ref="H86" r:id="rId77"/>
+    <hyperlink ref="H87" r:id="rId78"/>
+    <hyperlink ref="H88" r:id="rId79"/>
+    <hyperlink ref="H89" r:id="rId80"/>
+    <hyperlink ref="H90" r:id="rId81"/>
+    <hyperlink ref="H91" r:id="rId82"/>
+    <hyperlink ref="H92" r:id="rId83"/>
+    <hyperlink ref="H93" r:id="rId84"/>
+    <hyperlink ref="H94" r:id="rId85"/>
+    <hyperlink ref="H95" r:id="rId86"/>
+    <hyperlink ref="H96" r:id="rId87"/>
+    <hyperlink ref="H97" r:id="rId88"/>
+    <hyperlink ref="H98" r:id="rId89"/>
+    <hyperlink ref="H99" r:id="rId90"/>
+    <hyperlink ref="H100" r:id="rId91"/>
+    <hyperlink ref="H101" r:id="rId92"/>
+    <hyperlink ref="H102" r:id="rId93"/>
+    <hyperlink ref="H103" r:id="rId94"/>
+    <hyperlink ref="H104" r:id="rId95"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId96"/>
@@ -33382,7 +33381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33591,7 +33590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -34597,7 +34596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -35689,11 +35688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35940,20 +35939,23 @@
         <v>2</v>
       </c>
       <c r="C11" s="105">
-        <v>1</v>
+        <f>C9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="D11" s="105">
-        <v>1</v>
+        <f t="shared" ref="D11:E11" si="0">D9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="E11" s="105">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.75439886948727197</v>
       </c>
       <c r="F11" s="106" t="str">
         <f>'ISIC Code Mapping'!G2</f>
         <v>ISIC 27</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -35964,20 +35966,23 @@
         <v>3</v>
       </c>
       <c r="C12" s="105">
-        <v>0</v>
+        <f>C10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="D12" s="105">
-        <v>0</v>
+        <f t="shared" ref="D12:E12" si="1">D10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="E12" s="105">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.24560113051272803</v>
       </c>
       <c r="F12" s="106" t="str">
         <f>'ISIC Code Mapping'!G3</f>
         <v>ISIC 41T43</v>
       </c>
       <c r="G12" s="106" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -36106,7 +36111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -36121,7 +36126,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -37043,7 +37048,7 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
@@ -37067,7 +37072,7 @@
       </c>
       <c r="W7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>

</xml_diff>

<commit_message>
Split ISIC code 05T06
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
+++ b/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\SoBCaICbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\bldgs\SoBCaICbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DDD6A-EE2B-467B-813D-2B7069B42CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4448133-E82C-4976-9599-9CCDC816C525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="585" windowWidth="24090" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1725" yWindow="435" windowWidth="26295" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="624">
   <si>
     <t>Notes</t>
   </si>
@@ -2219,6 +2219,12 @@
   </si>
   <si>
     <t>ISIC 21</t>
+  </si>
+  <si>
+    <t>ISIC 05</t>
+  </si>
+  <si>
+    <t>ISIC 06</t>
   </si>
 </sst>
 </file>
@@ -3525,7 +3531,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3534,7 +3540,7 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>617</v>
       </c>
@@ -3542,115 +3548,118 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>622</v>
       </c>
       <c r="D1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>620</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>621</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>57</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>59</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>70</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>74</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -3724,11 +3733,11 @@
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="U2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -3744,11 +3753,11 @@
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Z2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -3802,8 +3811,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM2">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -3877,11 +3890,11 @@
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="U3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -3897,11 +3910,11 @@
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Z3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -3955,8 +3968,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM3">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -4108,8 +4125,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM4">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -4179,11 +4200,11 @@
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4261,8 +4282,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM5">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -4332,11 +4357,11 @@
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="T6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4356,11 +4381,11 @@
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Z6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -4414,8 +4439,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM6">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -4485,11 +4514,11 @@
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="T7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4509,11 +4538,11 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Z7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -4565,6 +4594,10 @@
       </c>
       <c r="AL7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -4578,7 +4611,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4587,7 +4620,7 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>617</v>
       </c>
@@ -4595,115 +4628,118 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>622</v>
       </c>
       <c r="D1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>620</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>621</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>57</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>59</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>70</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>74</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -4777,11 +4813,11 @@
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.70398750275034405</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.70398750275034405</v>
       </c>
       <c r="U2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -4797,11 +4833,11 @@
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.29601249724965595</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.29601249724965595</v>
       </c>
       <c r="Z2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -4855,8 +4891,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM2">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -4930,11 +4970,11 @@
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.5798301102469372</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.5798301102469372</v>
       </c>
       <c r="U3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -4950,11 +4990,11 @@
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.4201698897530628</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.4201698897530628</v>
       </c>
       <c r="Z3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -5008,8 +5048,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM3">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -5161,8 +5205,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM4">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -5232,11 +5280,11 @@
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.40766894664785691</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.40766894664785691</v>
       </c>
       <c r="T5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -5256,11 +5304,11 @@
       </c>
       <c r="X5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.59233105335214309</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.59233105335214309</v>
       </c>
       <c r="Z5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -5314,8 +5362,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM5">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -5385,11 +5437,11 @@
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.75439886948727197</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="T6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -5409,11 +5461,11 @@
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.24560113051272803</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Z6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -5467,8 +5519,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM6">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -5538,11 +5594,11 @@
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.75439886948727197</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="T7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -5562,11 +5618,11 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.24560113051272803</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Z7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -5618,6 +5674,10 @@
       </c>
       <c r="AL7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -36177,7 +36237,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36186,7 +36246,7 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>617</v>
       </c>
@@ -36194,115 +36254,118 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>622</v>
       </c>
       <c r="D1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>620</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>621</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>57</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>59</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>70</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>74</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -36376,11 +36439,11 @@
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="U2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -36396,11 +36459,11 @@
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Z2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -36454,8 +36517,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM2">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -36529,11 +36596,11 @@
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="U3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!U$1)</f>
@@ -36549,11 +36616,11 @@
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Z3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -36607,8 +36674,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM3">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -36760,8 +36831,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM4">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -36831,11 +36906,11 @@
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -36913,8 +36988,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM5">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -36984,11 +37063,11 @@
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="T6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -37008,11 +37087,11 @@
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Z6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -37066,8 +37145,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM6">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -37137,11 +37220,11 @@
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="T7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -37161,11 +37244,11 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Z7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Z$1)</f>
@@ -37217,6 +37300,10 @@
       </c>
       <c r="AL7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AM$1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>